<commit_message>
uso com um critério
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/6.Funcoes_Mercado/3.CONT.SES/1.Funcao_CONT.SES.xlsx
+++ b/2.Excel/hands-on/6.Funcoes_Mercado/3.CONT.SES/1.Funcao_CONT.SES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaof\Desktop\Excel Impressionador 2021\Módulo 8 - Funções Mercado de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\6.Funcoes_Mercado\3.CONT.SES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E79C64-1286-485D-968C-EE0DC01F6608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A210F975-F96A-4502-98D3-592E258F198C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3D2557DA-CD0B-48AD-8EFD-8912689B8782}"/>
+    <workbookView xWindow="12024" yWindow="96" windowWidth="10896" windowHeight="12792" activeTab="1" xr2:uid="{3D2557DA-CD0B-48AD-8EFD-8912689B8782}"/>
   </bookViews>
   <sheets>
     <sheet name="CONT.SES" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="92">
   <si>
     <t>Registro</t>
   </si>
@@ -515,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -531,17 +531,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -550,6 +550,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,9 +575,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -609,7 +615,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -715,7 +721,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -857,7 +863,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -865,18 +871,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37263547-D7E7-4AC6-B262-BC90CCAE7898}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.77734375" customWidth="1"/>
     <col min="2" max="4" width="15.77734375" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>70</v>
       </c>
@@ -890,7 +899,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -903,8 +912,14 @@
       <c r="D2" s="14">
         <v>11555</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -917,8 +932,12 @@
       <c r="D3" s="14">
         <v>23113</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3" s="16">
+        <f>COUNTIFS(B2:B14,F2,C2:C14,G2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -932,7 +951,7 @@
         <v>2585</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -946,7 +965,7 @@
         <v>32635</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -960,7 +979,7 @@
         <v>22529</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -974,12 +993,12 @@
         <v>33740</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
         <v>89</v>
@@ -988,7 +1007,7 @@
         <v>44566</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -1002,12 +1021,12 @@
         <v>16756</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
         <v>90</v>
@@ -1016,7 +1035,7 @@
         <v>24899</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -1030,7 +1049,7 @@
         <v>25086</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -1044,7 +1063,7 @@
         <v>6318</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -1058,7 +1077,7 @@
         <v>15710</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -1073,6 +1092,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{491133F9-BA05-4358-B616-952C83EC92BF}">
+      <formula1>"Amarela,Azul,Preta"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2 G2" xr:uid="{BD67C9FA-7B09-40B8-894A-66931606103C}">
+      <formula1>"Masculino,Feminino"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1081,7 +1108,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29FEF772-DFD0-4036-8B65-DBF82BF00CE4}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1173,7 +1202,10 @@
       <c r="E4" s="5">
         <v>42811</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7">
+        <f>COUNTIFS(B:B,"Coordenador")</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1252,7 +1284,10 @@
       <c r="E8" s="5">
         <v>42925</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7">
+        <f>COUNTIFS(E:E,"&gt;31/12/2018")</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">

</xml_diff>